<commit_message>
finish leftovers for output_pages
</commit_message>
<xml_diff>
--- a/src/output_template.xlsx
+++ b/src/output_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msv/codeforfun/spreadsheets-thing/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59217444-9616-B04E-B185-3F6ACD979733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978ABC73-341A-3E43-A1A5-B8274E265C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="880" windowWidth="31920" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="880" windowWidth="31920" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTENTS" sheetId="5" r:id="rId1"/>
@@ -1458,6 +1458,28 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
@@ -1916,7 +1938,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -2075,19 +2097,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2095,7 +2104,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2151,9 +2160,6 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2184,25 +2190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2255,6 +2243,24 @@
     <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2285,6 +2291,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2294,36 +2330,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2333,6 +2339,36 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2342,42 +2378,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2390,14 +2390,14 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3680,47 +3680,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B82379-4121-4CFA-8199-6B8591110E73}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" style="38" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="42" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="38" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="38"/>
+    <col min="1" max="1" width="32.1640625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="35" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="31" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="57"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56"/>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="55"/>
+      <c r="B3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3752,201 +3752,201 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="43" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="43" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="43" customWidth="1"/>
-    <col min="4" max="6" width="22" style="43" customWidth="1"/>
-    <col min="7" max="16384" width="9.83203125" style="43"/>
+    <col min="1" max="1" width="7.5" style="36" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="36" customWidth="1"/>
+    <col min="4" max="6" width="22" style="36" customWidth="1"/>
+    <col min="7" max="16384" width="9.83203125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="58"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E4" s="44"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
     </row>
     <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57" t="s">
+      <c r="B7" s="56"/>
+      <c r="C7" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="56" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="57"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:6" s="12" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+      <c r="A10" s="39"/>
     </row>
     <row r="11" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="60" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
     </row>
     <row r="13" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="48">
+      <c r="A13" s="41">
         <v>1</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="41">
         <v>2</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="41">
         <v>3</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="41">
         <v>4</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="41">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="47">
+      <c r="A14" s="40">
         <v>1</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="49" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="47">
-        <f>SUM(OUTPUT_PAGE!G14:G15)</f>
+      <c r="D14" s="40">
+        <f>SUM(OUTPUT_PAGE!G14:G14)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="47">
-        <f>SUM(OUTPUT_PAGE!H14:H15)</f>
+      <c r="E14" s="40">
+        <f>SUM(OUTPUT_PAGE!H14:H14)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="50" t="e">
-        <f>OUTPUT_PAGE!I15</f>
+      <c r="F14" s="43" t="e">
+        <f>OUTPUT_PAGE!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="54"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="54"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="36" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="36" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3982,14 +3982,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="107" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <pane xSplit="14" ySplit="12" topLeftCell="O13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8:G11"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4027,46 +4027,46 @@
     <row r="2" spans="1:21" s="6" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
-      <c r="O2" s="65" t="s">
+      <c r="O2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
     </row>
     <row r="3" spans="1:21" s="6" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="65" t="s">
+      <c r="O3" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="67" t="s">
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
     </row>
     <row r="4" spans="1:21" s="6" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
-      <c r="O4" s="65" t="s">
+      <c r="O4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="66" t="s">
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
     </row>
     <row r="5" spans="1:21" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
@@ -4083,42 +4083,42 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="68" t="s">
+      <c r="O5" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="68"/>
-      <c r="Q5" s="68"/>
-      <c r="R5" s="68"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
     </row>
     <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="71" t="s">
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="71"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="O7" s="14"/>
@@ -4130,110 +4130,110 @@
       <c r="U7" s="14"/>
     </row>
     <row r="8" spans="1:21" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="78" t="s">
+      <c r="F8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="81" t="s">
+      <c r="G8" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="84" t="s">
+      <c r="I8" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="85"/>
-      <c r="N8" s="86"/>
-      <c r="O8" s="90" t="s">
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="91"/>
-      <c r="Q8" s="91"/>
-      <c r="R8" s="91"/>
-      <c r="S8" s="91"/>
-      <c r="T8" s="92"/>
+      <c r="P8" s="85"/>
+      <c r="Q8" s="85"/>
+      <c r="R8" s="85"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="86"/>
       <c r="U8" s="12"/>
     </row>
     <row r="9" spans="1:21" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="73"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="93"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="94"/>
-      <c r="T9" s="95"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="88"/>
+      <c r="S9" s="88"/>
+      <c r="T9" s="89"/>
     </row>
     <row r="10" spans="1:21" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="73"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="96" t="s">
+      <c r="A10" s="69"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="98" t="s">
+      <c r="J10" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="99"/>
-      <c r="N10" s="100"/>
-      <c r="O10" s="101" t="s">
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="96"/>
+      <c r="O10" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="98" t="s">
+      <c r="P10" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="99"/>
-      <c r="R10" s="99"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="100"/>
+      <c r="Q10" s="96"/>
+      <c r="R10" s="96"/>
+      <c r="S10" s="96"/>
+      <c r="T10" s="99"/>
     </row>
     <row r="11" spans="1:21" ht="66.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="74"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="97"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="94"/>
       <c r="J11" s="15" t="s">
         <v>22</v>
       </c>
@@ -4246,10 +4246,10 @@
       <c r="M11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="102"/>
+      <c r="O11" s="98"/>
       <c r="P11" s="15" t="s">
         <v>22</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>1</v>
       </c>
@@ -4306,191 +4306,120 @@
       <c r="M12" s="16">
         <v>13</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="53">
         <v>14</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="17">
         <v>15</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12" s="17">
         <v>16</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="17">
         <v>17</v>
       </c>
-      <c r="R12" s="16">
+      <c r="R12" s="17">
         <v>18</v>
       </c>
-      <c r="S12" s="16">
+      <c r="S12" s="17">
         <v>19</v>
       </c>
-      <c r="T12" s="16">
+      <c r="T12" s="17">
         <v>20</v>
       </c>
       <c r="U12" s="12"/>
     </row>
-    <row r="13" spans="1:21" s="28" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25" t="e">
-        <f>SUM(O13+#REF!+#REF!+#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="26" t="e">
-        <f>P13+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K13" s="26" t="e">
-        <f>Q13+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L13" s="26" t="e">
-        <f>R13+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M13" s="26" t="e">
-        <f>S13+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N13" s="26" t="e">
-        <f>T13+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O13" s="27">
-        <f>SUM(P13:T13)</f>
+    <row r="13" spans="1:21" s="27" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24" cm="1">
+        <f t="array" ref="I13">SUMPRODUCT((MOD(COLUMN(O13:ZZ13)-COLUMN(O13),6)=0)*O13:ZZ13)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
+      <c r="J13" s="25" cm="1">
+        <f t="array" ref="J13">SUMPRODUCT((MOD(COLUMN(P13:ZZ13)-COLUMN(P13),6)=0)*P13:ZZ13)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="25" cm="1">
+        <f t="array" ref="K13">SUMPRODUCT((MOD(COLUMN(Q13:ZZ13)-COLUMN(Q13),6)=0)*Q13:ZZ13)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="25" cm="1">
+        <f t="array" ref="L13">SUMPRODUCT((MOD(COLUMN(R13:ZZ13)-COLUMN(R13),6)=0)*R13:ZZ13)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="25" cm="1">
+        <f t="array" ref="M13">SUMPRODUCT((MOD(COLUMN(S13:ZZ13)-COLUMN(S13),6)=0)*S13:ZZ13)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="25" cm="1">
+        <f t="array" ref="N13">SUMPRODUCT((MOD(COLUMN(T13:ZZ13)-COLUMN(T13),6)=0)*T13:ZZ13)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="26"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="14" spans="1:21" s="37" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34" t="e">
-        <f>SUM(O14+#REF!+#REF!+#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" s="35" t="e">
-        <f>P14+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K14" s="35" t="e">
-        <f>Q14+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L14" s="35" t="e">
-        <f>R14+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M14" s="35" t="e">
-        <f>S14+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N14" s="35" t="e">
-        <f>T14+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O14" s="36">
-        <f>SUM(P14:T14)</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="12"/>
-    </row>
-    <row r="15" spans="1:21" s="37" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34" t="e">
-        <f>SUM(O15+#REF!+#REF!+#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J15" s="35" t="e">
-        <f>P15+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K15" s="35" t="e">
-        <f>Q15+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L15" s="35" t="e">
-        <f>R15+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M15" s="35" t="e">
-        <f>S15+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N15" s="35" t="e">
-        <f>T15+#REF!+#REF!++#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O15" s="36">
-        <f>SUM(P15:T15)</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="32">
-        <f>P14-G15</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="12"/>
+    <row r="14" spans="1:21" s="30" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="49"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="24">
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="P10:T10"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="S4:U4"/>
     <mergeCell ref="O5:R5"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="B8:B11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="I8:N9"/>
+    <mergeCell ref="O8:T9"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="F8:F11"/>
     <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="I8:N9"/>
-    <mergeCell ref="O8:T9"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:N10"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="S4:U4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" location="Зміст!A1" display="Повернутись на зміст" xr:uid="{DC1D9212-3194-4FD6-8CE0-21807E23B2A5}"/>

</xml_diff>

<commit_message>
Lamost finish generating pages
</commit_message>
<xml_diff>
--- a/src/output_template.xlsx
+++ b/src/output_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msv/codeforfun/spreadsheets-thing/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978ABC73-341A-3E43-A1A5-B8274E265C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC385162-3E5A-3F4C-9A99-B1CBAD5D7095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="880" windowWidth="31920" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="880" windowWidth="31920" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTENTS" sheetId="5" r:id="rId1"/>
@@ -1358,7 +1358,7 @@
     <definedName name="яяя" localSheetId="1" hidden="1">{#N/A,#N/A,TRUE,"Ком";#N/A,#N/A,TRUE,"ALL"}</definedName>
     <definedName name="яяя" hidden="1">{#N/A,#N/A,TRUE,"Ком";#N/A,#N/A,TRUE,"ALL"}</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="1" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1374,110 +1374,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Admin</author>
-  </authors>
-  <commentList>
-    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{4315FFEC-AB82-41F7-A6C1-36FA2A5FD0E1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>За ціником 2003 року (радянські боєприпаси)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P14" authorId="0" shapeId="0" xr:uid="{CA551711-D28C-434B-8246-D4D70B4C4648}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Тут надійшло</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1689,7 +1585,7 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1896,21 +1792,6 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2151,18 +2032,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2258,9 +2127,21 @@
     <xf numFmtId="165" fontId="22" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2291,36 +2172,105 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2329,75 +2279,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3680,16 +3561,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B82379-4121-4CFA-8199-6B8591110E73}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="35" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="31" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="31"/>
+    <col min="1" max="1" width="32.1640625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="31" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3710,17 +3591,17 @@
     </row>
     <row r="3" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="55"/>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="28" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3747,16 +3628,16 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="36" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="36" customWidth="1"/>
-    <col min="4" max="6" width="22" style="36" customWidth="1"/>
-    <col min="7" max="16384" width="9.83203125" style="36"/>
+    <col min="1" max="1" width="7.5" style="32" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="32" customWidth="1"/>
+    <col min="4" max="6" width="22" style="32" customWidth="1"/>
+    <col min="7" max="16384" width="9.83203125" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3774,7 +3655,7 @@
       <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E4" s="37"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="58" t="s">
@@ -3825,11 +3706,11 @@
       <c r="B9" s="62"/>
       <c r="C9" s="63"/>
       <c r="D9" s="63"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
+      <c r="A10" s="35"/>
     </row>
     <row r="11" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="60" t="s">
@@ -3860,61 +3741,52 @@
       <c r="F12" s="60"/>
     </row>
     <row r="13" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41">
+      <c r="A13" s="37">
         <v>1</v>
       </c>
-      <c r="B13" s="41">
+      <c r="B13" s="37">
         <v>2</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="37">
         <v>3</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="37">
         <v>4</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="37">
         <v>5</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="37">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="40">
+      <c r="A14" s="36">
         <v>1</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="42" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="40">
-        <f>SUM(OUTPUT_PAGE!G14:G14)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="40">
-        <f>SUM(OUTPUT_PAGE!H14:H14)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="43" t="e">
-        <f>OUTPUT_PAGE!#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="61" t="s">
@@ -3926,10 +3798,10 @@
       <c r="E18" s="61"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="32" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3943,10 +3815,10 @@
       <c r="E21" s="61"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="32" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3976,7 +3848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37014A25-B80E-441D-864E-0370B6A8B897}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37014A25-B80E-441D-864E-0370B6A8B897}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3984,12 +3856,12 @@
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="92" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <pane xSplit="14" ySplit="12" topLeftCell="O13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4027,46 +3899,46 @@
     <row r="2" spans="1:21" s="6" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
-      <c r="O2" s="74" t="s">
+      <c r="O2" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
     </row>
     <row r="3" spans="1:21" s="6" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="74" t="s">
+      <c r="O3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="76" t="s">
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
     </row>
     <row r="4" spans="1:21" s="6" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
-      <c r="O4" s="74" t="s">
+      <c r="O4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="75" t="s">
+      <c r="P4" s="97"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
+      <c r="T4" s="98"/>
+      <c r="U4" s="98"/>
     </row>
     <row r="5" spans="1:21" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
@@ -4083,42 +3955,42 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="64" t="s">
+      <c r="O5" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
+      <c r="S5" s="96"/>
+      <c r="T5" s="96"/>
+      <c r="U5" s="96"/>
     </row>
     <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="67" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="65"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="O7" s="14"/>
@@ -4130,110 +4002,110 @@
       <c r="U7" s="14"/>
     </row>
     <row r="8" spans="1:21" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="90" t="s">
+      <c r="G8" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="80" t="s">
+      <c r="I8" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="84" t="s">
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="85"/>
-      <c r="Q8" s="85"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85"/>
-      <c r="T8" s="86"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="80"/>
+      <c r="T8" s="81"/>
       <c r="U8" s="12"/>
     </row>
     <row r="9" spans="1:21" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="69"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="87"/>
-      <c r="P9" s="88"/>
-      <c r="Q9" s="88"/>
-      <c r="R9" s="88"/>
-      <c r="S9" s="88"/>
-      <c r="T9" s="89"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="83"/>
+      <c r="R9" s="83"/>
+      <c r="S9" s="83"/>
+      <c r="T9" s="84"/>
     </row>
     <row r="10" spans="1:21" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="93" t="s">
+      <c r="A10" s="67"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="95" t="s">
+      <c r="J10" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
-      <c r="N10" s="96"/>
-      <c r="O10" s="97" t="s">
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="95" t="s">
+      <c r="P10" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-      <c r="S10" s="96"/>
-      <c r="T10" s="99"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="94"/>
     </row>
     <row r="11" spans="1:21" ht="66.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="70"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="94"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="89"/>
       <c r="J11" s="15" t="s">
         <v>22</v>
       </c>
@@ -4246,10 +4118,10 @@
       <c r="M11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="48" t="s">
+      <c r="N11" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="98"/>
+      <c r="O11" s="93"/>
       <c r="P11" s="15" t="s">
         <v>22</v>
       </c>
@@ -4266,146 +4138,86 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
-        <v>1</v>
-      </c>
-      <c r="B12" s="16">
-        <v>2</v>
-      </c>
-      <c r="C12" s="16">
-        <v>3</v>
-      </c>
-      <c r="D12" s="16">
-        <v>4</v>
-      </c>
-      <c r="E12" s="16">
-        <v>5</v>
-      </c>
-      <c r="F12" s="16">
-        <v>6</v>
-      </c>
-      <c r="G12" s="16">
-        <v>7</v>
-      </c>
-      <c r="H12" s="17">
-        <v>8</v>
-      </c>
-      <c r="I12" s="18">
-        <v>9</v>
-      </c>
-      <c r="J12" s="16">
-        <v>10</v>
-      </c>
-      <c r="K12" s="16">
-        <v>11</v>
-      </c>
-      <c r="L12" s="16">
-        <v>12</v>
-      </c>
-      <c r="M12" s="16">
-        <v>13</v>
-      </c>
-      <c r="N12" s="53">
-        <v>14</v>
-      </c>
-      <c r="O12" s="17">
-        <v>15</v>
-      </c>
-      <c r="P12" s="17">
-        <v>16</v>
-      </c>
-      <c r="Q12" s="17">
-        <v>17</v>
-      </c>
-      <c r="R12" s="17">
-        <v>18</v>
-      </c>
-      <c r="S12" s="17">
-        <v>19</v>
-      </c>
-      <c r="T12" s="17">
-        <v>20</v>
-      </c>
+    <row r="12" spans="1:21" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
       <c r="U12" s="12"/>
     </row>
-    <row r="13" spans="1:21" s="27" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24" cm="1">
-        <f t="array" ref="I13">SUMPRODUCT((MOD(COLUMN(O13:ZZ13)-COLUMN(O13),6)=0)*O13:ZZ13)</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="25" cm="1">
-        <f t="array" ref="J13">SUMPRODUCT((MOD(COLUMN(P13:ZZ13)-COLUMN(P13),6)=0)*P13:ZZ13)</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="25" cm="1">
-        <f t="array" ref="K13">SUMPRODUCT((MOD(COLUMN(Q13:ZZ13)-COLUMN(Q13),6)=0)*Q13:ZZ13)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="25" cm="1">
-        <f t="array" ref="L13">SUMPRODUCT((MOD(COLUMN(R13:ZZ13)-COLUMN(R13),6)=0)*R13:ZZ13)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="25" cm="1">
-        <f t="array" ref="M13">SUMPRODUCT((MOD(COLUMN(S13:ZZ13)-COLUMN(S13),6)=0)*S13:ZZ13)</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="25" cm="1">
-        <f t="array" ref="N13">SUMPRODUCT((MOD(COLUMN(T13:ZZ13)-COLUMN(T13),6)=0)*T13:ZZ13)</f>
-        <v>0</v>
-      </c>
-      <c r="O13" s="26"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
+    <row r="13" spans="1:21" s="23" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="14" spans="1:21" s="30" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="49"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="49"/>
+    <row r="14" spans="1:21" s="26" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="45"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="24">
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="S5:U5"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="O3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="S4:U4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="S5:U5"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A8:A11"/>
@@ -4420,6 +4232,8 @@
     <mergeCell ref="G8:G11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:N10"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:T10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" location="Зміст!A1" display="Повернутись на зміст" xr:uid="{DC1D9212-3194-4FD6-8CE0-21807E23B2A5}"/>
@@ -4429,6 +4243,5 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="14" max="1048575" man="1"/>
   </colBreaks>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix the last template OMG
</commit_message>
<xml_diff>
--- a/src/output_template.xlsx
+++ b/src/output_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msv/codeforfun/spreadsheets-thing/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F503850-E9CF-8B4A-BD9D-F8976EC28289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA7BCB0-BE32-7542-B3F4-851C73B447CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="880" windowWidth="31920" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="880" windowWidth="31920" windowHeight="25700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTENTS" sheetId="5" r:id="rId1"/>
@@ -1994,6 +1994,9 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2062,9 +2065,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3360,23 +3360,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:3" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="44"/>
     </row>
     <row r="3" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="18" t="s">
         <v>31</v>
       </c>
@@ -3411,10 +3411,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3426,107 +3426,133 @@
     <col min="7" max="16384" width="9.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="44" t="s">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="44"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
+    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E4" s="23"/>
+      <c r="G4" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
     </row>
-    <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43" t="s">
+      <c r="D7" s="44"/>
+      <c r="E7" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
     </row>
-    <row r="9" spans="1:6" s="12" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
+    <row r="9" spans="1:11" s="12" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="25"/>
     </row>
-    <row r="11" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+    <row r="11" spans="1:11" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
     </row>
-    <row r="13" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27">
         <v>1</v>
       </c>
@@ -3546,7 +3572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
         <v>1</v>
       </c>
@@ -3558,7 +3584,7 @@
       <c r="E14" s="26"/>
       <c r="F14" s="29"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="30"/>
       <c r="B15" s="11"/>
       <c r="C15" s="31"/>
@@ -3566,7 +3592,7 @@
       <c r="E15" s="32"/>
       <c r="F15" s="33"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="30"/>
       <c r="B16" s="11"/>
       <c r="C16" s="31"/>
@@ -3574,46 +3600,12 @@
       <c r="E16" s="32"/>
       <c r="F16" s="33"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>50</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G4:K4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="A11:A12"/>
@@ -3642,7 +3634,7 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="55" zoomScaleSheetLayoutView="92" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="92" zoomScaleNormal="55" zoomScaleSheetLayoutView="92" workbookViewId="0">
       <pane xSplit="14" ySplit="12" topLeftCell="O13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
@@ -3713,15 +3705,15 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="61" t="s">
+      <c r="O2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
     </row>
     <row r="3" spans="1:21" ht="19.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -3740,17 +3732,17 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="61" t="s">
+      <c r="O3" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="63" t="s">
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
     </row>
     <row r="4" spans="1:21" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -3767,17 +3759,17 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
-      <c r="O4" s="61" t="s">
+      <c r="O4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="61"/>
-      <c r="S4" s="62" t="s">
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
     </row>
     <row r="5" spans="1:21" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
@@ -3794,42 +3786,42 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
     </row>
     <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="O7" s="14"/>
@@ -3841,112 +3833,112 @@
       <c r="U7"/>
     </row>
     <row r="8" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="55" t="s">
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
       <c r="U8"/>
     </row>
     <row r="9" spans="1:21" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
       <c r="U9"/>
     </row>
     <row r="10" spans="1:21" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="57" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="J10" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="58" t="s">
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="43" t="s">
+      <c r="P10" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
       <c r="U10"/>
     </row>
     <row r="11" spans="1:21" ht="66.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="57"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="58"/>
       <c r="J11" s="15" t="s">
         <v>22</v>
       </c>
@@ -3962,7 +3954,7 @@
       <c r="N11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="58"/>
+      <c r="O11" s="59"/>
       <c r="P11" s="15" t="s">
         <v>22</v>
       </c>
@@ -4005,11 +3997,11 @@
     </row>
     <row r="13" spans="1:21" s="39" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="37"/>

</xml_diff>